<commit_message>
Added backup and restore configuration
</commit_message>
<xml_diff>
--- a/export/excel/facts.xlsx
+++ b/export/excel/facts.xlsx
@@ -425,10 +425,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="40" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
@@ -498,7 +498,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>10:36:00</t>
+          <t>8:54:00</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>11:40:13</t>
+          <t>12:08:00</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -562,17 +562,17 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>9LVB3XPUL11</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>Version 15.0(TTC_20140605)FLO_DSGS7</t>
+          <t>Version 15.2(4.0.55)E</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>11:35:00</t>
+          <t>12:04:00</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Refactor juniper ip_routes export
</commit_message>
<xml_diff>
--- a/export/excel/facts.xlsx
+++ b/export/excel/facts.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G4"/>
+  <dimension ref="A2:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>6:58:00</t>
+          <t>2:50:00</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -510,35 +510,72 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>R3.automation.local</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Juniper</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>12.1R1.9</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>4:43:56</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
           <t>SW1</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>SW1.automation.local</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Cisco</t>
         </is>
       </c>
-      <c r="D4" s="1" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>9DXW0R8PLH0</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>Version 15.2(4.0.55)E</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>11:59:00</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>4:42:00</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>

<commit_message>
Packet filter refactor (viewer, exporter)
</commit_message>
<xml_diff>
--- a/export/excel/facts.xlsx
+++ b/export/excel/facts.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G5"/>
+  <dimension ref="A2:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,9 +428,10 @@
     <col width="30" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="30" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -451,20 +452,25 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
           <t>serial_number</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>os_version</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>uptime</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>connection</t>
         </is>
@@ -488,20 +494,25 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
+          <t>7206VXR</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
           <t>4279256517</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>Version 15.2(4)S5</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>2:50:00</t>
-        </is>
-      </c>
       <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>5:00:00</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -525,20 +536,25 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
+          <t>OLIVE</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>12.1R1.9</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>4:43:56</t>
-        </is>
-      </c>
       <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>8:28:32</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -562,20 +578,25 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
+          <t>IOSv</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
           <t>9DXW0R8PLH0</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>Version 15.2(4.0.55)E</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>4:42:00</t>
-        </is>
-      </c>
       <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>8:26:00</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>

<commit_message>
Finished docs, only yaml docs missing
</commit_message>
<xml_diff>
--- a/export/excel/facts.xlsx
+++ b/export/excel/facts.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>5:00:00</t>
+          <t>0:07:00</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>8:28:32</t>
+          <t>0:11:21</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>9DXW0R8PLH0</t>
+          <t>9K3RW05NXRW</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>8:26:00</t>
+          <t>0:11:00</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Finished, except monitoring and yaml comments, examples
</commit_message>
<xml_diff>
--- a/export/excel/facts.xlsx
+++ b/export/excel/facts.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>0:07:00</t>
+          <t>3:41:00</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>0:11:21</t>
+          <t>6:19:37</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>0:11:00</t>
+          <t>6:18:00</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Final - without vault pass
</commit_message>
<xml_diff>
--- a/export/excel/facts.xlsx
+++ b/export/excel/facts.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H5"/>
+  <dimension ref="A2:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,7 +509,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>3:41:00</t>
+          <t>5:36:00</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -521,12 +521,12 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R2</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>R3.automation.local</t>
+          <t>R2.automation.local</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>6:19:37</t>
+          <t>5:42:22</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -563,12 +563,12 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SW1</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>SW1.automation.local</t>
+          <t>R3.automation.local</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -578,25 +578,67 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
+          <t>7206VXR</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>4279256517</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>Version 15.2(4)S5</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>5:34:00</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>MLS1</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>MLS1.automation.local</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>Cisco</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
           <t>IOSv</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>9K3RW05NXRW</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>9LD1YQMD0KM</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
         <is>
           <t>Version 15.2(4.0.55)E</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>6:18:00</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>5:42:00</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>